<commit_message>
created api test cases of login app_version
</commit_message>
<xml_diff>
--- a/exec/symlex_vpn_windows/api_test_cases/email_verification/username_field__positive.xlsx
+++ b/exec/symlex_vpn_windows/api_test_cases/email_verification/username_field__positive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\exec\symlex_vpn_windows\api_test_cases\email_verification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1053B2BA-CD9D-44C2-9F9F-93C9A2A6DBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2057D6C-E509-4B1C-908E-53E8CF540E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,22 +143,13 @@
     <t>test username field with a mix of uppercase and lowercase letters</t>
   </si>
   <si>
-    <t>verify username field with a mix of letters, numbers, and special characters</t>
-  </si>
-  <si>
     <t>SYM-API-SP-021</t>
-  </si>
-  <si>
-    <t>verify username field with a mix of alphanumeric characters and spaces</t>
   </si>
   <si>
     <t>SYM-API-SP-022</t>
   </si>
   <si>
     <t>SYM-API-SP-023</t>
-  </si>
-  <si>
-    <t>test username field with boundary values (minimum and maximum length)</t>
   </si>
   <si>
     <t>SYM-API-SP-024</t>
@@ -170,9 +161,6 @@
     <t>SYM-API-SP-026</t>
   </si>
   <si>
-    <t>verify username field with valid username and password combination</t>
-  </si>
-  <si>
     <t>should return a successful response with status code 200
 (actual result : 422 status code)</t>
   </si>
@@ -181,15 +169,6 @@
   </si>
   <si>
     <t>verify username field with valid email format containing underscores in the local part</t>
-  </si>
-  <si>
-    <t>verify username field with valid email format containing multiple subdomains</t>
-  </si>
-  <si>
-    <t>verify username field with valid email format containing leading and trailing spaces</t>
-  </si>
-  <si>
-    <t>verify username field with valid email format containing a hyphen at the beginning of the local part</t>
   </si>
   <si>
     <t>1. open the postman
@@ -445,6 +424,36 @@
   <si>
     <t>verify with valid email format but using unicode characters
 Input: "उदाहरण@example.com"</t>
+  </si>
+  <si>
+    <t>verify username field with a mix of letters, numbers, and special characters
+Input: "user123!@example.com"</t>
+  </si>
+  <si>
+    <t>verify username field with valid email format containing multiple subdomains
+Input: "user@mail.example.co.uk"</t>
+  </si>
+  <si>
+    <t>verify username field with a mix of alphanumeric characters and spaces
+Input: "user name123@example.com"</t>
+  </si>
+  <si>
+    <t>test username field with boundary values (minimum and maximum length)
+Input: "a@example.com"
+Input: "abcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyz@example.com"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify username field with valid username and password combination
+Input: "example_user123@example.com"
+</t>
+  </si>
+  <si>
+    <t>verify username field with valid email format containing leading and trailing spaces
+Input: " user123@example.com "</t>
+  </si>
+  <si>
+    <t>verify username field with valid email format containing a hyphen at the beginning of the local part
+Input: "-user123@example.com"</t>
   </si>
 </sst>
 </file>
@@ -1889,8 +1898,8 @@
   <dimension ref="A1:Z979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1907,7 +1916,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -2016,13 +2025,13 @@
         <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>8</v>
@@ -2058,13 +2067,13 @@
         <v>32</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="3"/>
@@ -2098,13 +2107,13 @@
         <v>34</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="3"/>
@@ -2135,16 +2144,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="3"/>
@@ -2178,13 +2187,13 @@
         <v>35</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -2215,10 +2224,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>33</v>
@@ -2255,13 +2264,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>7</v>
@@ -2295,16 +2304,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
@@ -2335,16 +2344,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -2375,16 +2384,16 @@
         <v>9</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
@@ -2418,13 +2427,13 @@
         <v>37</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
@@ -2458,13 +2467,13 @@
         <v>38</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="1"/>
@@ -2498,13 +2507,13 @@
         <v>39</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="1"/>
@@ -2535,16 +2544,16 @@
         <v>9</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="1"/>
@@ -2575,16 +2584,16 @@
         <v>9</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="1"/>
@@ -2615,16 +2624,16 @@
         <v>9</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="1"/>
@@ -2655,16 +2664,16 @@
         <v>9</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="1"/>
@@ -2695,16 +2704,16 @@
         <v>9</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="1"/>
@@ -2735,16 +2744,16 @@
         <v>9</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="1"/>
@@ -2775,16 +2784,16 @@
         <v>9</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E23" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="1"/>
@@ -2809,22 +2818,22 @@
     </row>
     <row r="24" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="1"/>
@@ -2849,16 +2858,16 @@
     </row>
     <row r="25" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>33</v>
@@ -2887,24 +2896,24 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="189" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="1"/>
@@ -2929,22 +2938,22 @@
     </row>
     <row r="27" spans="1:26" ht="129" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="1"/>
@@ -2969,22 +2978,22 @@
     </row>
     <row r="28" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="1"/>
@@ -3009,22 +3018,22 @@
     </row>
     <row r="29" spans="1:26" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="1"/>

</xml_diff>